<commit_message>
pegue lander, pegue o test_started 012
</commit_message>
<xml_diff>
--- a/FlaskServer/Resultados.xlsx
+++ b/FlaskServer/Resultados.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>Nome</t>
   </si>
@@ -45,12 +45,24 @@
   </si>
   <si>
     <t>% de acertos</t>
+  </si>
+  <si>
+    <t>Vitória</t>
+  </si>
+  <si>
+    <t>18/10/2005</t>
+  </si>
+  <si>
+    <t>02:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0%"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -68,7 +80,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,6 +90,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF123499"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF39E75F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7F7F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -109,9 +133,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -408,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -467,6 +503,38 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3">
+        <v>500</v>
+      </c>
+      <c r="D3" s="4">
+        <v>750</v>
+      </c>
+      <c r="E3" s="4">
+        <v>100</v>
+      </c>
+      <c r="F3" s="3">
+        <v>200</v>
+      </c>
+      <c r="G3" s="4">
+        <v>900</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="2">
+        <v>15</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -482,7 +550,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -541,6 +609,38 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4">
+        <v>164</v>
+      </c>
+      <c r="D3" s="4">
+        <v>234</v>
+      </c>
+      <c r="E3" s="4">
+        <v>987</v>
+      </c>
+      <c r="F3" s="4">
+        <v>433</v>
+      </c>
+      <c r="G3" s="4">
+        <v>765</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="2">
+        <v>15</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Fixed a server error
</commit_message>
<xml_diff>
--- a/FlaskServer/Resultados.xlsx
+++ b/FlaskServer/Resultados.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="13">
   <si>
     <t>Nome</t>
   </si>
@@ -444,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -533,6 +533,70 @@
         <v>15</v>
       </c>
       <c r="J3" s="5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3">
+        <v>500</v>
+      </c>
+      <c r="D4" s="4">
+        <v>750</v>
+      </c>
+      <c r="E4" s="4">
+        <v>100</v>
+      </c>
+      <c r="F4" s="3">
+        <v>200</v>
+      </c>
+      <c r="G4" s="4">
+        <v>900</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="2">
+        <v>15</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
+        <v>500</v>
+      </c>
+      <c r="D5" s="4">
+        <v>750</v>
+      </c>
+      <c r="E5" s="4">
+        <v>100</v>
+      </c>
+      <c r="F5" s="3">
+        <v>200</v>
+      </c>
+      <c r="G5" s="4">
+        <v>900</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="2">
+        <v>15</v>
+      </c>
+      <c r="J5" s="5">
         <v>0.4</v>
       </c>
     </row>
@@ -550,7 +614,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -639,6 +703,70 @@
         <v>15</v>
       </c>
       <c r="J3" s="5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4">
+        <v>164</v>
+      </c>
+      <c r="D4" s="4">
+        <v>234</v>
+      </c>
+      <c r="E4" s="4">
+        <v>987</v>
+      </c>
+      <c r="F4" s="4">
+        <v>433</v>
+      </c>
+      <c r="G4" s="4">
+        <v>765</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="2">
+        <v>15</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4">
+        <v>164</v>
+      </c>
+      <c r="D5" s="4">
+        <v>234</v>
+      </c>
+      <c r="E5" s="4">
+        <v>987</v>
+      </c>
+      <c r="F5" s="4">
+        <v>433</v>
+      </c>
+      <c r="G5" s="4">
+        <v>765</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="2">
+        <v>15</v>
+      </c>
+      <c r="J5" s="5">
         <v>0.4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added minimum value for minutes
</commit_message>
<xml_diff>
--- a/FlaskServer/Resultados.xlsx
+++ b/FlaskServer/Resultados.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>Nome</t>
   </si>
@@ -45,12 +45,24 @@
   </si>
   <si>
     <t>% de acertos</t>
+  </si>
+  <si>
+    <t>Vitória Jaqueline Lopes Zago</t>
+  </si>
+  <si>
+    <t>18/10/2005</t>
+  </si>
+  <si>
+    <t>02:35:10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0%"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -68,7 +80,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,6 +90,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF123499"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF39E75F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7F7F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -109,9 +133,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -408,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -479,6 +515,38 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3">
+        <v>500</v>
+      </c>
+      <c r="D3" s="4">
+        <v>750</v>
+      </c>
+      <c r="E3" s="4">
+        <v>100</v>
+      </c>
+      <c r="F3" s="3">
+        <v>200</v>
+      </c>
+      <c r="G3" s="4">
+        <v>900</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="2">
+        <v>15</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.4</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
@@ -493,7 +561,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -564,6 +632,38 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4">
+        <v>164</v>
+      </c>
+      <c r="D3" s="4">
+        <v>234</v>
+      </c>
+      <c r="E3" s="4">
+        <v>987</v>
+      </c>
+      <c r="F3" s="4">
+        <v>433</v>
+      </c>
+      <c r="G3" s="4">
+        <v>765</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="2">
+        <v>15</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.4</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A2"/>

</xml_diff>

<commit_message>
Post HTTP req done
</commit_message>
<xml_diff>
--- a/FlaskServer/Resultados.xlsx
+++ b/FlaskServer/Resultados.xlsx
@@ -47,13 +47,13 @@
     <t>% de acertos</t>
   </si>
   <si>
-    <t>Vitória Jaqueline Lopes Zago</t>
-  </si>
-  <si>
-    <t>18/10/2005</t>
-  </si>
-  <si>
-    <t>02:35:10</t>
+    <t>OH KAMI OH MY GOD</t>
+  </si>
+  <si>
+    <t>12/12/2012</t>
+  </si>
+  <si>
+    <t>00:43:20</t>
   </si>
 </sst>
 </file>
@@ -525,23 +525,23 @@
       <c r="C3" s="3">
         <v>500</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="3">
         <v>750</v>
       </c>
-      <c r="E3" s="4">
-        <v>100</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
+        <v>300</v>
+      </c>
+      <c r="G3" s="4">
         <v>200</v>
-      </c>
-      <c r="G3" s="4">
-        <v>900</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J3" s="5">
         <v>0.4</v>
@@ -640,25 +640,25 @@
         <v>11</v>
       </c>
       <c r="C3" s="4">
-        <v>164</v>
+        <v>0</v>
       </c>
       <c r="D3" s="4">
-        <v>234</v>
+        <v>676</v>
       </c>
       <c r="E3" s="4">
-        <v>987</v>
+        <v>600</v>
       </c>
       <c r="F3" s="4">
-        <v>433</v>
+        <v>80</v>
       </c>
       <c r="G3" s="4">
-        <v>765</v>
+        <v>40</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J3" s="5">
         <v>0.4</v>

</xml_diff>

<commit_message>
Timer and fixes for new json
</commit_message>
<xml_diff>
--- a/FlaskServer/Resultados.xlsx
+++ b/FlaskServer/Resultados.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Nome</t>
   </si>
@@ -45,24 +45,12 @@
   </si>
   <si>
     <t>% de acertos</t>
-  </si>
-  <si>
-    <t>OH KAMI OH MY GOD</t>
-  </si>
-  <si>
-    <t>12/12/2012</t>
-  </si>
-  <si>
-    <t>00:43:20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0%"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -80,7 +68,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -90,18 +78,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF123499"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF39E75F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF7F7F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -133,21 +109,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -444,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -515,38 +479,6 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3">
-        <v>500</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1000</v>
-      </c>
-      <c r="E3" s="3">
-        <v>750</v>
-      </c>
-      <c r="F3" s="4">
-        <v>300</v>
-      </c>
-      <c r="G3" s="4">
-        <v>200</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0.4</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
@@ -561,7 +493,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -632,38 +564,6 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>676</v>
-      </c>
-      <c r="E3" s="4">
-        <v>600</v>
-      </c>
-      <c r="F3" s="4">
-        <v>80</v>
-      </c>
-      <c r="G3" s="4">
-        <v>40</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0.4</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A2"/>

</xml_diff>